<commit_message>
again some lines for Rende~
</commit_message>
<xml_diff>
--- a/output/reporthouronfcst.xlsx
+++ b/output/reporthouronfcst.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,50 +441,45 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>Attesa</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Attesa</t>
+          <t>Risposte Eff.</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Risposte Eff.</t>
+          <t>Offerte</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Offerte</t>
+          <t>Abb sup. 14</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Abb sup. 14</t>
+          <t>Abb inf. 14</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Abb inf. 14</t>
+          <t>Short Call min 10</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Short Call min 10</t>
+          <t>Cleared</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Cleared</t>
+          <t>10/03/2023</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>10/03/2023</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Delta_Offerto</t>
         </is>
@@ -497,34 +492,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>855</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>329</v>
       </c>
       <c r="D2" t="n">
-        <v>313</v>
+        <v>334</v>
       </c>
       <c r="E2" t="n">
-        <v>316</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H2" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>318.5</v>
       </c>
       <c r="J2" t="n">
-        <v>200.2</v>
-      </c>
-      <c r="K2" t="n">
-        <v>57.84215784215785</v>
+        <v>4.866562009419151</v>
       </c>
     </row>
     <row r="3">
@@ -534,34 +526,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>851</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>155</v>
       </c>
       <c r="D3" t="n">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="E3" t="n">
-        <v>166</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
         <v>2</v>
       </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
       <c r="H3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>206</v>
       </c>
       <c r="J3" t="n">
-        <v>147</v>
-      </c>
-      <c r="K3" t="n">
-        <v>12.9251700680272</v>
+        <v>-24.75728155339806</v>
       </c>
     </row>
     <row r="4">
@@ -571,16 +560,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>762</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D4" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -592,13 +581,10 @@
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J4" t="n">
-        <v>2</v>
-      </c>
-      <c r="K4" t="n">
-        <v>250</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5">
@@ -608,34 +594,31 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>852</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>153</v>
       </c>
       <c r="D5" t="n">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="E5" t="n">
-        <v>170</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="J5" t="n">
-        <v>74</v>
-      </c>
-      <c r="K5" t="n">
-        <v>129.7297297297297</v>
+        <v>46.22641509433962</v>
       </c>
     </row>
     <row r="6">
@@ -645,16 +628,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>765</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D6" t="n">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -666,13 +649,10 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="J6" t="n">
-        <v>33</v>
-      </c>
-      <c r="K6" t="n">
-        <v>-75.75757575757575</v>
+        <v>-36.8421052631579</v>
       </c>
     </row>
     <row r="7">
@@ -682,34 +662,31 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2189</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D7" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E7" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="J7" t="n">
-        <v>56</v>
-      </c>
-      <c r="K7" t="n">
-        <v>-71.42857142857143</v>
+        <v>-69.51219512195121</v>
       </c>
     </row>
     <row r="8">
@@ -719,34 +696,31 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5207</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>159</v>
       </c>
       <c r="D8" t="n">
-        <v>113</v>
+        <v>164</v>
       </c>
       <c r="E8" t="n">
-        <v>122</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J8" t="n">
-        <v>23</v>
-      </c>
-      <c r="K8" t="n">
-        <v>430.4347826086956</v>
+        <v>613.0434782608695</v>
       </c>
     </row>
     <row r="9">
@@ -756,34 +730,31 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3092</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D9" t="n">
         <v>17</v>
       </c>
       <c r="E9" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="J9" t="n">
-        <v>58</v>
-      </c>
-      <c r="K9" t="n">
-        <v>-68.96551724137932</v>
+        <v>-70.68965517241379</v>
       </c>
     </row>
     <row r="10">
@@ -793,34 +764,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2072</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="D10" t="n">
-        <v>84</v>
+        <v>178</v>
       </c>
       <c r="E10" t="n">
-        <v>90</v>
+        <v>23</v>
       </c>
       <c r="F10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>379</v>
       </c>
       <c r="J10" t="n">
-        <v>270</v>
-      </c>
-      <c r="K10" t="n">
-        <v>-66.66666666666667</v>
+        <v>-53.03430079155673</v>
       </c>
     </row>
     <row r="11">
@@ -830,34 +798,31 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>845</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="D11" t="n">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="E11" t="n">
-        <v>113</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="J11" t="n">
-        <v>175</v>
-      </c>
-      <c r="K11" t="n">
-        <v>-35.42857142857143</v>
+        <v>-39.42307692307693</v>
       </c>
     </row>
     <row r="12">
@@ -867,34 +832,31 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2347</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>18</v>
+        <v>217</v>
       </c>
       <c r="D12" t="n">
-        <v>132</v>
+        <v>270</v>
       </c>
       <c r="E12" t="n">
-        <v>259</v>
+        <v>11</v>
       </c>
       <c r="F12" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H12" t="n">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="I12" t="n">
-        <v>71</v>
+        <v>395.2</v>
       </c>
       <c r="J12" t="n">
-        <v>258.7</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0.1159644375724911</v>
+        <v>-31.68016194331984</v>
       </c>
     </row>
     <row r="13">
@@ -904,19 +866,19 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>703</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D13" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -925,13 +887,10 @@
         <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>302</v>
       </c>
       <c r="J13" t="n">
-        <v>220</v>
-      </c>
-      <c r="K13" t="n">
-        <v>-97.72727272727273</v>
+        <v>-96.35761589403974</v>
       </c>
     </row>
     <row r="14">
@@ -941,34 +900,31 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>847</v>
+        <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>13</v>
+        <v>298</v>
       </c>
       <c r="D14" t="n">
-        <v>134</v>
+        <v>314</v>
       </c>
       <c r="E14" t="n">
-        <v>203</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="G14" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H14" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I14" t="n">
-        <v>17</v>
+        <v>495</v>
       </c>
       <c r="J14" t="n">
-        <v>353</v>
-      </c>
-      <c r="K14" t="n">
-        <v>-42.49291784702549</v>
+        <v>-36.56565656565657</v>
       </c>
     </row>
     <row r="15">
@@ -978,34 +934,31 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1614</v>
+        <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="D15" t="n">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="E15" t="n">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="J15" t="n">
-        <v>92</v>
-      </c>
-      <c r="K15" t="n">
-        <v>-23.91304347826086</v>
+        <v>-30.70866141732284</v>
       </c>
     </row>
     <row r="16">
@@ -1015,34 +968,31 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1739</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="D16" t="n">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="E16" t="n">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="F16" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H16" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>134</v>
       </c>
       <c r="J16" t="n">
-        <v>134</v>
-      </c>
-      <c r="K16" t="n">
-        <v>-30.59701492537313</v>
+        <v>-24.6268656716418</v>
       </c>
     </row>
     <row r="17">
@@ -1052,34 +1002,31 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2793</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="D17" t="n">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="E17" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="J17" t="n">
-        <v>50</v>
-      </c>
-      <c r="K17" t="n">
-        <v>-64</v>
+        <v>-57.14285714285714</v>
       </c>
     </row>
     <row r="18">
@@ -1089,19 +1036,19 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>681</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" t="n">
         <v>1</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
@@ -1110,15 +1057,10 @@
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="n">
         <v>0</v>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
       </c>
     </row>
     <row r="19">
@@ -1128,16 +1070,16 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>717</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D19" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -1149,13 +1091,10 @@
         <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J19" t="n">
-        <v>6</v>
-      </c>
-      <c r="K19" t="n">
-        <v>-16.66666666666666</v>
+        <v>-22.22222222222222</v>
       </c>
     </row>
     <row r="20">
@@ -1165,16 +1104,16 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2246</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E20" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -1186,13 +1125,10 @@
         <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="J20" t="n">
-        <v>28</v>
-      </c>
-      <c r="K20" t="n">
-        <v>-57.14285714285714</v>
+        <v>-50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>